<commit_message>
3rd dataset DT, LR and Simple RF
</commit_message>
<xml_diff>
--- a/Banking dataset Decision Tree/Performance_metrics/model_perf_metrics_mean_of_iterations_1356_2712_4069__1_2 .xlsx
+++ b/Banking dataset Decision Tree/Performance_metrics/model_perf_metrics_mean_of_iterations_1356_2712_4069__1_2 .xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,7 +490,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -502,16 +502,16 @@
         <v>31647</v>
       </c>
       <c r="G2" t="n">
-        <v>0.5032828579986734</v>
+        <v>0.5028938270292095</v>
       </c>
       <c r="H2" t="n">
-        <v>0.00165948</v>
+        <v>0.00407062</v>
       </c>
       <c r="I2" t="n">
-        <v>0.690136704725467</v>
+        <v>0.6900002850299007</v>
       </c>
       <c r="J2" t="n">
-        <v>0.00018247</v>
+        <v>0.00210366</v>
       </c>
     </row>
     <row r="3">
@@ -524,7 +524,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -558,7 +558,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -570,16 +570,16 @@
         <v>31647</v>
       </c>
       <c r="G4" t="n">
-        <v>0.4772858656385724</v>
+        <v>0.4846250348041683</v>
       </c>
       <c r="H4" t="n">
-        <v>0.00146134</v>
+        <v>0.00568506</v>
       </c>
       <c r="I4" t="n">
-        <v>0.7104336291432111</v>
+        <v>0.7150502036319386</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0009907500000000001</v>
+        <v>0.00392709</v>
       </c>
     </row>
     <row r="5">
@@ -588,32 +588,32 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>DT_sample:10_cf:1_mean_of_2_iterations</t>
+          <t>DT_sample:1356_cf:1_mean_of_5_iterations</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D5" t="n">
-        <v>10</v>
+        <v>1356</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>31657</v>
+        <v>33003</v>
       </c>
       <c r="G5" t="n">
-        <v>0.4830339611501975</v>
+        <v>0.4672272462712558</v>
       </c>
       <c r="H5" t="n">
-        <v>0.00288153</v>
+        <v>0.008394789999999999</v>
       </c>
       <c r="I5" t="n">
-        <v>0.7142730093128038</v>
+        <v>0.7008665457116703</v>
       </c>
       <c r="J5" t="n">
-        <v>0.00107629</v>
+        <v>0.00599623</v>
       </c>
     </row>
     <row r="6">
@@ -622,32 +622,168 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>DT_sample:10_cf:2_mean_of_2_iterations</t>
+          <t>DT_sample:1356_cf:2_mean_of_5_iterations</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>10</v>
+        <v>1356</v>
       </c>
       <c r="E6" t="n">
         <v>2</v>
       </c>
       <c r="F6" t="n">
-        <v>31667</v>
+        <v>34359</v>
       </c>
       <c r="G6" t="n">
-        <v>0.4837231623264986</v>
+        <v>0.4610902867966988</v>
       </c>
       <c r="H6" t="n">
-        <v>0.00269422</v>
+        <v>0.00714374</v>
       </c>
       <c r="I6" t="n">
-        <v>0.7138631692036155</v>
+        <v>0.6934237462795376</v>
       </c>
       <c r="J6" t="n">
-        <v>0.00202215</v>
+        <v>0.00477817</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>DT_sample:2712_cf:1_mean_of_5_iterations</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2712</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>34359</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.4637420381395428</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.00327374</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.6960786134391599</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.00174809</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>DT_sample:2712_cf:2_mean_of_5_iterations</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>5</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2712</v>
+      </c>
+      <c r="E8" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" t="n">
+        <v>37071</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.4586469228887627</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.00432843</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.6899385212429496</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.00272537</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>DT_sample:4069_cf:1_mean_of_5_iterations</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>5</v>
+      </c>
+      <c r="D9" t="n">
+        <v>4069</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" t="n">
+        <v>35716</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.4655479305685267</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.01236409</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.6949310611334323</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.0067427</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>DT_sample:4069_cf:2_mean_of_5_iterations</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>5</v>
+      </c>
+      <c r="D10" t="n">
+        <v>4069</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" t="n">
+        <v>39785</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.4577977849919957</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.00696073</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.6864653332383234</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.00334761</v>
       </c>
     </row>
   </sheetData>

</xml_diff>